<commit_message>
Update processed and raw data files
Added Community_Composition.csv and removed Compos10m2.csv and Compos1m2.csv in processed data. Updated BC_2025_Cover_Data.csv header, Sampling5.0Data.csv, trait_joined_finCharly.xlsx, traits.csv, and made changes to data_wrangling.R to reflect new data structure and content.
</commit_message>
<xml_diff>
--- a/data/raw_data/trait_joined_finCharly.xlsx
+++ b/data/raw_data/trait_joined_finCharly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62d82b30bc78fab5/Documents/BIOLOGIE/Blooming Campus/A_Paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oksana\Nextcloud\2026\Manuscripts\Guttek_et_al\Guttek_et_al_2026\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{2254E2A0-066F-496A-8F32-D6DDBB0571F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AACF5D7-2885-4443-8B34-BCBD99179269}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555660E9-CD24-4C1F-B60D-346B0C9E8CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trait_joined" sheetId="1" r:id="rId1"/>
@@ -1266,17 +1266,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1367,10 +1363,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1709,32 +1701,32 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.53515625" customWidth="1"/>
-    <col min="2" max="2" width="25.3046875" customWidth="1"/>
-    <col min="3" max="3" width="16.53515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.53515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="26.765625" customWidth="1"/>
-    <col min="7" max="7" width="17.23046875" customWidth="1"/>
-    <col min="8" max="8" width="22.53515625" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="11" width="18.61328125" customWidth="1"/>
-    <col min="12" max="12" width="20.4609375" customWidth="1"/>
-    <col min="13" max="13" width="20.15234375" customWidth="1"/>
-    <col min="14" max="14" width="12.921875" customWidth="1"/>
-    <col min="15" max="15" width="14.23046875" customWidth="1"/>
-    <col min="16" max="16" width="18.07421875" customWidth="1"/>
-    <col min="17" max="17" width="16.4609375" customWidth="1"/>
-    <col min="18" max="18" width="18.3046875" customWidth="1"/>
-    <col min="19" max="19" width="16.765625" customWidth="1"/>
-    <col min="20" max="20" width="19.3828125" customWidth="1"/>
-    <col min="21" max="21" width="17.4609375" customWidth="1"/>
+    <col min="11" max="11" width="18.6328125" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="12.90625" customWidth="1"/>
+    <col min="15" max="15" width="14.26953125" customWidth="1"/>
+    <col min="16" max="16" width="18.08984375" customWidth="1"/>
+    <col min="17" max="17" width="16.453125" customWidth="1"/>
+    <col min="18" max="18" width="18.26953125" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" customWidth="1"/>
+    <col min="20" max="20" width="19.36328125" customWidth="1"/>
+    <col min="21" max="21" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1799,7 +1791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1864,7 +1856,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -1929,11 +1921,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>227</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1994,7 +1986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -2059,7 +2051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2124,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2189,14 +2181,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2254,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>148</v>
       </c>
@@ -2319,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -2384,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2449,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>206</v>
       </c>
@@ -2514,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>212</v>
       </c>
@@ -2579,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>152</v>
       </c>
@@ -2644,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -2709,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -2774,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>218</v>
       </c>
@@ -2839,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>202</v>
       </c>
@@ -2904,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2969,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -3034,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -3099,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -3164,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>211</v>
       </c>
@@ -3229,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -3294,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -3359,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -3424,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3489,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -3554,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -3619,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -3684,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -3749,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3814,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -3879,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3944,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -4009,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -4074,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -4139,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -4204,7 +4196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -4269,8 +4261,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>83</v>
       </c>
       <c r="B40" t="s">
@@ -4334,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -4399,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>210</v>
       </c>
@@ -4464,8 +4456,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>97</v>
       </c>
       <c r="B43" t="s">
@@ -4529,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>120</v>
       </c>
@@ -4594,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>127</v>
       </c>
@@ -4659,8 +4651,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>128</v>
       </c>
       <c r="B46" t="s">
@@ -4724,8 +4716,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>160</v>
       </c>
       <c r="B47" t="s">
@@ -4789,8 +4781,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>214</v>
       </c>
       <c r="B48" t="s">
@@ -4854,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>159</v>
       </c>
@@ -4919,7 +4911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>164</v>
       </c>
@@ -4984,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -5049,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -5114,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -5179,7 +5171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>183</v>
       </c>
@@ -5244,7 +5236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -5309,7 +5301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>199</v>
       </c>
@@ -5374,7 +5366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -5439,7 +5431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -5504,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>200</v>
       </c>
@@ -5569,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -5634,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -5699,7 +5691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -5764,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -5829,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -5894,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -5959,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -6024,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -6089,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -6154,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -6219,7 +6211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -6284,7 +6276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -6349,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>205</v>
       </c>
@@ -6414,8 +6406,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A73" s="6" t="s">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>42</v>
       </c>
       <c r="B73" t="s">
@@ -6479,7 +6471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -6544,7 +6536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -6609,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>54</v>
       </c>
@@ -6674,7 +6666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -6739,7 +6731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>59</v>
       </c>
@@ -6804,7 +6796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>56</v>
       </c>
@@ -6869,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -6934,7 +6926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>61</v>
       </c>
@@ -6999,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>62</v>
       </c>
@@ -7064,7 +7056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>63</v>
       </c>
@@ -7129,7 +7121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>65</v>
       </c>
@@ -7194,7 +7186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>72</v>
       </c>
@@ -7259,7 +7251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -7324,7 +7316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -7389,7 +7381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -7454,7 +7446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -7519,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -7584,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -7649,7 +7641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -7714,7 +7706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>81</v>
       </c>
@@ -7724,7 +7716,7 @@
       <c r="C93" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="D93" s="2" t="s">
         <v>223</v>
       </c>
       <c r="E93">
@@ -7779,7 +7771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>84</v>
       </c>
@@ -7844,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>85</v>
       </c>
@@ -7909,7 +7901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -7974,7 +7966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>91</v>
       </c>
@@ -8039,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>92</v>
       </c>
@@ -8104,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>93</v>
       </c>
@@ -8169,7 +8161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>94</v>
       </c>
@@ -8234,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>95</v>
       </c>
@@ -8299,8 +8291,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A102" s="6" t="s">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>96</v>
       </c>
       <c r="B102" t="s">
@@ -8364,8 +8356,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A103" s="6" t="s">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>98</v>
       </c>
       <c r="B103" t="s">
@@ -8429,8 +8421,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A104" s="6" t="s">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>99</v>
       </c>
       <c r="B104" t="s">
@@ -8494,8 +8486,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A105" s="6" t="s">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>100</v>
       </c>
       <c r="B105" t="s">
@@ -8559,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -8624,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -8689,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>104</v>
       </c>
@@ -8754,7 +8746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -8819,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>106</v>
       </c>
@@ -8884,7 +8876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -8949,7 +8941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>109</v>
       </c>
@@ -9014,7 +9006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -9079,7 +9071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -9144,7 +9136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>116</v>
       </c>
@@ -9209,7 +9201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -9274,8 +9266,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A117" s="6" t="s">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>118</v>
       </c>
       <c r="B117" t="s">
@@ -9339,7 +9331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>123</v>
       </c>
@@ -9404,7 +9396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>124</v>
       </c>
@@ -9469,7 +9461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -9534,7 +9526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>173</v>
       </c>
@@ -9599,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>134</v>
       </c>
@@ -9664,8 +9656,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A123" s="6" t="s">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>129</v>
       </c>
       <c r="B123" t="s">
@@ -9729,7 +9721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -9794,14 +9786,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>132</v>
       </c>
       <c r="B125" t="s">
         <v>132</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="C125" t="s">
         <v>232</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -9859,7 +9851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -9924,7 +9916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -9989,7 +9981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -10054,7 +10046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -10119,7 +10111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>139</v>
       </c>
@@ -10184,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>140</v>
       </c>
@@ -10249,7 +10241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>142</v>
       </c>
@@ -10314,7 +10306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>143</v>
       </c>
@@ -10379,7 +10371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>215</v>
       </c>
@@ -10444,7 +10436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>144</v>
       </c>
@@ -10509,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>146</v>
       </c>
@@ -10574,7 +10566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -10639,7 +10631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -10704,7 +10696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -10769,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>217</v>
       </c>
@@ -10834,7 +10826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -10899,7 +10891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>86</v>
       </c>
@@ -10964,7 +10956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>89</v>
       </c>
@@ -11029,7 +11021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>111</v>
       </c>
@@ -11094,7 +11086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>162</v>
       </c>
@@ -11159,7 +11151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -11224,7 +11216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>165</v>
       </c>
@@ -11289,7 +11281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>166</v>
       </c>
@@ -11354,8 +11346,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A149" s="6" t="s">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>167</v>
       </c>
       <c r="B149" t="s">
@@ -11419,7 +11411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>121</v>
       </c>
@@ -11484,7 +11476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>170</v>
       </c>
@@ -11549,7 +11541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>171</v>
       </c>
@@ -11614,14 +11606,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>172</v>
       </c>
       <c r="B153" t="s">
         <v>172</v>
       </c>
-      <c r="C153" s="7" t="s">
+      <c r="C153" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D153" s="2" t="s">
@@ -11679,7 +11671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>175</v>
       </c>
@@ -11744,7 +11736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>176</v>
       </c>
@@ -11809,7 +11801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>177</v>
       </c>
@@ -11874,7 +11866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>178</v>
       </c>
@@ -11939,7 +11931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>180</v>
       </c>
@@ -12004,7 +11996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>182</v>
       </c>
@@ -12069,7 +12061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>186</v>
       </c>
@@ -12134,7 +12126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>187</v>
       </c>
@@ -12199,7 +12191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>188</v>
       </c>
@@ -12264,7 +12256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>189</v>
       </c>
@@ -12329,7 +12321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>192</v>
       </c>
@@ -12394,7 +12386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>193</v>
       </c>
@@ -12459,7 +12451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>195</v>
       </c>
@@ -12524,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>196</v>
       </c>
@@ -12589,7 +12581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>197</v>
       </c>
@@ -12654,8 +12646,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A169" s="6" t="s">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
         <v>194</v>
       </c>
       <c r="B169" t="s">
@@ -12719,7 +12711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>198</v>
       </c>
@@ -12784,7 +12776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>45</v>
       </c>
@@ -12849,14 +12841,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>52</v>
       </c>
       <c r="B172" t="s">
         <v>52</v>
       </c>
-      <c r="C172" s="7" t="s">
+      <c r="C172" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D172" s="2" t="s">
@@ -12914,14 +12906,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>53</v>
       </c>
       <c r="B173" t="s">
         <v>53</v>
       </c>
-      <c r="C173" s="7" t="s">
+      <c r="C173" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D173" s="2" t="s">
@@ -12979,7 +12971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>71</v>
       </c>
@@ -13044,14 +13036,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>50</v>
       </c>
       <c r="B175" t="s">
         <v>51</v>
       </c>
-      <c r="C175" s="7" t="s">
+      <c r="C175" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D175" s="2" t="s">
@@ -13109,7 +13101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>209</v>
       </c>
@@ -13174,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>101</v>
       </c>
@@ -13239,7 +13231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>154</v>
       </c>
@@ -13304,7 +13296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>158</v>
       </c>
@@ -13369,8 +13361,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A180" s="6" t="s">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>185</v>
       </c>
       <c r="B180" t="s">

</xml_diff>